<commit_message>
ajout dans repartition tache, idées de plot, support de cours, date soutenance etc
</commit_message>
<xml_diff>
--- a/repartition_taches.xlsx
+++ b/repartition_taches.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="32" uniqueCount="25">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="75" uniqueCount="65">
   <si>
     <t>Leila</t>
   </si>
@@ -102,13 +102,135 @@
   </si>
   <si>
     <t>exploration bdd, stat desc</t>
+  </si>
+  <si>
+    <t>IDEES PLOT</t>
+  </si>
+  <si>
+    <t>LIENS SUPPORTS DE COURS</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1DyO7neGVnJft3ynPk1m1vjaV2MG_JOFOp5gmJMdcY-4/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>cours 1</t>
+  </si>
+  <si>
+    <t>intro avec les dataviz de l'an passé</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1DEaGNHEaz3uGnX5Vhv4SBDtdCagngSerna3cx-gYyg0/edit?usp=sharing </t>
+  </si>
+  <si>
+    <t>toolbox pour faire graphes interactifs</t>
+  </si>
+  <si>
+    <t>https://github.com/hachichaud/ensae-dataviz</t>
+  </si>
+  <si>
+    <t>Repo github de la prof avec exemples code dataviz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cours 2</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1EuhPa7n0TGslqmakHuN8D1xlFnhNhiMF-TaBP36Zgqs/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>PROCHAINS COURS</t>
+  </si>
+  <si>
+    <t>soutenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) trouver les 2, 3 histoires étonnantes (contextualiser données, croiser variables, zommez) (2) adapter squelette du site (3) premiers plot
+</t>
+  </si>
+  <si>
+    <t>avant dernier cours</t>
+  </si>
+  <si>
+    <t>45 Ways to Communicate Two Quantities</t>
+  </si>
+  <si>
+    <t>Pour ouvrir vos chacras sur les manières de représenter un même dataset</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/graphics/2016-who-marries-whom/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un exple intéressant (même si un peu trop exploratoire pour nous) </t>
+  </si>
+  <si>
+    <t>interactions entre volumes consommés et montants remboursés / non remboursés, Et la part de dépenses qui est remboursée / la part non remboursée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Et les «secteurs» de la santé qui sont en «essor» ? (ex antidépresseurs ? Certains types de spécialistes sont-ils de + en + consultés ces dernières années ? (depuis 2009) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Médicaments les + vendus par nb de boîtes (quizz) et «Sous-groupe thérapeutique» des médicaments les + vendus en nb de boîtes (ex : psychoanaleptique, «médicaments du rhume et de la toux»)</t>
+  </si>
+  <si>
+    <t>Médicaments pour lesquels les Frç ont dépensé le + en euros</t>
+  </si>
+  <si>
+    <t>Montants dépensés (et remboursés) pour les génériques / pour les non génériques</t>
+  </si>
+  <si>
+    <t>carte des dépenses de médicaments par région (seulement 13 régions en fait)</t>
+  </si>
+  <si>
+    <t>carte des montant des dépassements d’honoraires pour certains spécialistes</t>
+  </si>
+  <si>
+    <t>Evolution depuis 2009 des montants des dépassements d’honoraires</t>
+  </si>
+  <si>
+    <t>evolution</t>
+  </si>
+  <si>
+    <t>Spécialistes chez lesquels les Frç ont dépensé le + en dépassements d’honoraires ? (attention peut-être à l’effet «affichage» / «dénonciation»)</t>
+  </si>
+  <si>
+    <t>Les dépenses en homéopathie remboursée</t>
+  </si>
+  <si>
+    <t>On peut aussi faire un focus sur les vaccins les + achetés</t>
+  </si>
+  <si>
+    <t>evolution/barchart</t>
+  </si>
+  <si>
+    <t>consultation chez le médecin (par ex psy) par mois</t>
+  </si>
+  <si>
+    <t>NB : médicaments =&gt; vision annuelle, visite médecin =&gt; vision mensuelle (base DAMIR qui recense ensemble des actes remboursés mensuellement)</t>
+  </si>
+  <si>
+    <t>Problèmes :</t>
+  </si>
+  <si>
+    <t>dépassements d'honoraires et ya des chiffres vmt très hauts, plausible ?</t>
+  </si>
+  <si>
+    <t>medicaments</t>
+  </si>
+  <si>
+    <t>montants remboursés (REM) supérieurs à la base de remboursement (BSE)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +254,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF4B4F56"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF90949C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF4B4F56"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +293,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <start/>
       <end/>
@@ -170,12 +323,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -193,9 +403,53 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,14 +765,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="1" max="1" width="10.36328125" customWidth="1"/>
     <col min="2" max="2" width="25.453125" customWidth="1"/>
     <col min="3" max="3" width="25.6328125" customWidth="1"/>
     <col min="4" max="4" width="34.90625" customWidth="1"/>
@@ -526,205 +781,506 @@
     <col min="6" max="6" width="31.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18.5">
       <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.5">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="14" customHeight="1">
+      <c r="A3" s="18" t="d">
+        <v>2018-04-06</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="18" t="d">
+        <v>2018-04-13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="18" t="d">
+        <v>2018-04-27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.5">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E9" s="3">
         <v>4</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F9" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="7" t="s">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.5">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="19" spans="1:6">
+      <c r="A19" s="4">
         <v>1</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B19" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="52" customHeight="1">
+      <c r="A20" s="4">
         <v>2</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B20" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4">
         <v>3</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B21" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4">
         <v>4</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B22" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="29">
+      <c r="A23" s="4">
         <v>5</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.5">
+      <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18.5">
+      <c r="A26" s="7"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4">
+        <v>2</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4">
+        <v>3</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4">
+        <v>4</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4">
+        <v>5</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="4">
+        <v>6</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4">
+        <v>7</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4">
+        <v>8</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="4">
+        <v>9</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="4">
+        <v>10</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4">
+        <v>11</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="4">
+        <v>12</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="8"/>
+      <c r="B42" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="29">
+      <c r="A46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="29">
+      <c r="A47" s="12"/>
+      <c r="B47" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="29">
+      <c r="A48" s="13"/>
+      <c r="B48" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.5">
+      <c r="A50" s="22"/>
+      <c r="B50" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.5">
+      <c r="A51" s="22"/>
+      <c r="B51" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="29">
+      <c r="B58" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59" s="26"/>
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="D60" s="27"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="D61" s="28"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="D63" s="26"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="D64" s="26"/>
+    </row>
+    <row r="66" spans="4:4">
+      <c r="D66" s="26"/>
+    </row>
+    <row r="67" spans="4:4">
+      <c r="D67" s="26"/>
+    </row>
+    <row r="69" spans="4:4">
+      <c r="D69" s="26"/>
+    </row>
+    <row r="71" spans="4:4">
+      <c r="D71" s="26"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A49:A51"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" display="https://l.facebook.com/l.php?u=http%3A%2F%2Fwww.lemonde.fr%2Fles-decodeurs%2Farticle%2F2017%2F11%2F28%2Fmedicaments-et-remboursements-la-base-de-donnees-open-medic-en-6-points_5221378_4355770.html&amp;h=ATPtooBirJjDbGZaIxTe-cbdqBF8WbScXeLUhCKaUVy7coKuYAozODihAbPJ-DDNBIcNOIro2SX3PKPcGvXV7FcrdvLXaNo-aU4WM5N_rb5ZzT4iFLk"/>
+    <hyperlink ref="C20" r:id="rId1" display="https://l.facebook.com/l.php?u=http%3A%2F%2Fwww.lemonde.fr%2Fles-decodeurs%2Farticle%2F2017%2F11%2F28%2Fmedicaments-et-remboursements-la-base-de-donnees-open-medic-en-6-points_5221378_4355770.html&amp;h=ATPtooBirJjDbGZaIxTe-cbdqBF8WbScXeLUhCKaUVy7coKuYAozODihAbPJ-DDNBIcNOIro2SX3PKPcGvXV7FcrdvLXaNo-aU4WM5N_rb5ZzT4iFLk"/>
+    <hyperlink ref="C46" r:id="rId2"/>
+    <hyperlink ref="C47" r:id="rId3" display="https://docs.google.com/presentation/d/1DEaGNHEaz3uGnX5Vhv4SBDtdCagngSerna3cx-gYyg0/edit?usp=sharing"/>
+    <hyperlink ref="C48" r:id="rId4"/>
+    <hyperlink ref="C49" r:id="rId5"/>
+    <hyperlink ref="C50" r:id="rId6" tooltip="45 Ways to Communicate Two Quantities" display="https://visual.ly/blog/45-ways-to-communicate-two-quantities/"/>
+    <hyperlink ref="C51" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout article mort medic
</commit_message>
<xml_diff>
--- a/repartition_taches.xlsx
+++ b/repartition_taches.xlsx
@@ -62,9 +62,6 @@
     <t>article 1 : http://www.lemonde.fr/les-decodeurs/article/2017/11/28/medicaments-et-remboursements-la-base-de-donnees-open-medic-en-6-points_5221378_4355770.html</t>
   </si>
   <si>
-    <t>article 2 :</t>
-  </si>
-  <si>
     <t>article 3 :</t>
   </si>
   <si>
@@ -224,6 +221,10 @@
   </si>
   <si>
     <t>montants remboursés (REM) supérieurs à la base de remboursement (BSE)</t>
+  </si>
+  <si>
+    <t>article 2 :
+http://www.lemonde.fr/sante/article/2018/03/22/plus-de-10-000-morts-par-an-liees-a-mauvais-usage-des-medicaments_5274559_1651302.html</t>
   </si>
 </sst>
 </file>
@@ -385,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -407,15 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -429,12 +421,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -450,6 +436,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -767,8 +771,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -783,42 +787,42 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.5">
       <c r="A1" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.5">
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="14" customHeight="1">
-      <c r="A3" s="18" t="d">
+      <c r="A3" s="15" t="d">
         <v>2018-04-06</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="d">
+        <v>2018-04-13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="18" t="d">
-        <v>2018-04-13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="18" t="d">
+      <c r="A5" s="15" t="d">
         <v>2018-04-27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="16"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:6" ht="18.5">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -842,7 +846,7 @@
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -854,7 +858,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -911,7 +915,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -925,15 +929,15 @@
     </row>
     <row r="17" spans="1:6" ht="18.5">
       <c r="A17" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4">
         <v>1</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>24</v>
+      <c r="B19" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -948,17 +952,17 @@
       <c r="A20" s="4">
         <v>2</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="F20" s="5"/>
     </row>
@@ -966,14 +970,14 @@
       <c r="A21" s="4">
         <v>3</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -982,17 +986,17 @@
       <c r="A22" s="4">
         <v>4</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F22" s="5"/>
     </row>
@@ -1000,11 +1004,11 @@
       <c r="A23" s="4">
         <v>5</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1012,7 +1016,7 @@
     </row>
     <row r="25" spans="1:6" ht="18.5">
       <c r="A25" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18.5">
@@ -1020,123 +1024,123 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4">
         <v>2</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4">
         <v>3</v>
       </c>
-      <c r="B30" s="19"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4">
         <v>4</v>
       </c>
-      <c r="B31" s="19"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="4">
         <v>5</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4">
         <v>6</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>15</v>
+      <c r="B33" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4">
         <v>7</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>15</v>
+      <c r="B34" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4">
         <v>8</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>54</v>
+      <c r="B35" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4">
         <v>9</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4">
         <v>10</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4">
         <v>11</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4">
         <v>12</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1146,24 +1150,24 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="8"/>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="8"/>
@@ -1172,99 +1176,99 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="29">
+      <c r="A46" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="29">
-      <c r="A46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="20" t="s">
+    <row r="47" spans="1:4" ht="29">
+      <c r="A47" s="26"/>
+      <c r="B47" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="29">
-      <c r="A47" s="12"/>
-      <c r="B47" s="23" t="s">
+    </row>
+    <row r="48" spans="1:4" ht="29">
+      <c r="A48" s="27"/>
+      <c r="B48" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="29">
-      <c r="A48" s="13"/>
-      <c r="B48" s="23" t="s">
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="21" t="s">
+      <c r="B49" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="50" spans="1:4" ht="43.5">
-      <c r="A50" s="22"/>
-      <c r="B50" s="20" t="s">
+      <c r="A50" s="29"/>
+      <c r="B50" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.5">
+      <c r="A51" s="29"/>
+      <c r="B51" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="43.5">
-      <c r="A51" s="22"/>
-      <c r="B51" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="29">
       <c r="B58" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="B59" s="26"/>
-      <c r="D59" s="26"/>
+      <c r="B59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="D60" s="27"/>
+      <c r="D60" s="22"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="D61" s="28"/>
+      <c r="D61" s="23"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="D63" s="26"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="D64" s="26"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="66" spans="4:4">
-      <c r="D66" s="26"/>
+      <c r="D66" s="21"/>
     </row>
     <row r="67" spans="4:4">
-      <c r="D67" s="26"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="69" spans="4:4">
-      <c r="D69" s="26"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="71" spans="4:4">
-      <c r="D71" s="26"/>
+      <c r="D71" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
ajout des idées postées sur fb
</commit_message>
<xml_diff>
--- a/repartition_taches.xlsx
+++ b/repartition_taches.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Desktop\cours3A\semestre2\dataviz\dataviz\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
   <si>
     <t>PROCHAINS COURS</t>
   </si>
@@ -304,10 +309,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
     <t>Bleu plus foncé : base médicaments — années : 2014 à 2016</t>
   </si>
   <si>
@@ -315,13 +316,58 @@
   </si>
   <si>
     <t>Frise ? En passant le curseur le long de la frise, on verrait apparaître pour chaque année le médicament «gagnant» en montants dépensés totaux</t>
+  </si>
+  <si>
+    <t>les médicaments les plus chers mais seulement dans le champ des anti-dépresseurs. L’évolution depuis 2009 des dépassements d’honoraires mais seulement chez les psychiatres. Et la répartition des dépenses et des visites dans ce domaine en fonction des régions / départements.</t>
+  </si>
+  <si>
+    <t>IDEES</t>
+  </si>
+  <si>
+    <t>Une autre piste serait un focus sur les différences de consommation entre les hommes et les femmes en comparant par exemple les dépassements d’honoraires des urologues et des gyneco, ou un focus sur le prix des pilules (mais pas sure que les médicaments type « pilules » soient facilement identifiables)</t>
+  </si>
+  <si>
+    <t>d’après un article du Monde en 2016 les psychiatres étaient les 3e médecins spécialistes aux taux de dépassements d’honoraires les plus hauts. Du coup ce que j’ai commencé à regarder c’est quel type de « prestation » pour les psychiatres avaient les taux de dépassement les plus hauts. Genre est-ce que les forts taux de dépassements sont circonscrits à des consultations un peu exceptionnelles. Effectivement pour l’instant il s’avère que les prestations du type « avis de consultation donné auprès d’un hôpital » sont plus sujettes aux dépassements que les consultations mais bon j’ai juste bossé avec les chiffres de janvier 2018 pour l’instant haha</t>
+  </si>
+  <si>
+    <t>focus</t>
+  </si>
+  <si>
+    <t>Mais peut-être qu’une histoire pourrait être de dire « ok les psy sont parmi les champions des dépassements d’honoraires, mais quel type de prestations font-ils vraiment payer plus cher ? »</t>
+  </si>
+  <si>
+    <t>histoire</t>
+  </si>
+  <si>
+    <t>médicaments innovants</t>
+  </si>
+  <si>
+    <t>(il s'agit des nouveaux traitements souvent très cher pour des maladies graves type cancer, HIV ou hépatite C - ils sont bien entendu sous brevet, d'où leur coût)</t>
+  </si>
+  <si>
+    <r>
+      <t>bon en fait la définition est plus précise que ça (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://ansm.sante.fr/L-ANSM/Medicaments-de-therapie-innovante-et-preparations-cellulaires-a-finalite-therapeutique/Les-medicaments-de-therapie-innovante-MTI-ATMP/(offset)/4)</t>
+    </r>
+  </si>
+  <si>
+    <t>et ça fait débat pcq c'est très cher et pourrait poser des problèmes quant à l'égalité d'accès aux soins.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -366,6 +412,25 @@
       <color theme="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -405,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -620,16 +685,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -681,35 +812,12 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -741,13 +849,51 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Lien hypertexte visité" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -820,6 +966,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1901,18 +2055,18 @@
   <dimension ref="A1:IV70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" style="1" customWidth="1"/>
+    <col min="7" max="256" width="8.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" customHeight="1">
@@ -2216,7 +2370,7 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" ht="18.5" customHeight="1">
-      <c r="A26" s="51"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2224,192 +2378,192 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="18.5" customHeight="1">
-      <c r="A27" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
+      <c r="A27" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" ht="18.5" customHeight="1">
-      <c r="A28" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1">
-      <c r="A30" s="44">
+      <c r="A30" s="35">
         <v>1</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
     </row>
     <row r="31" spans="1:6" ht="16" customHeight="1">
-      <c r="A31" s="44">
+      <c r="A31" s="35">
         <v>2</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="42" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1">
-      <c r="A32" s="44">
+      <c r="A32" s="35">
         <v>3</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
     </row>
     <row r="33" spans="1:6" ht="81" customHeight="1">
-      <c r="A33" s="44">
+      <c r="A33" s="35">
         <v>4</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
     </row>
     <row r="34" spans="1:6" ht="16" customHeight="1">
-      <c r="A34" s="44">
+      <c r="A34" s="35">
         <v>5</v>
       </c>
       <c r="B34" s="22"/>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
     </row>
     <row r="35" spans="1:6" ht="16" customHeight="1">
-      <c r="A35" s="44">
+      <c r="A35" s="35">
         <v>6</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="55"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
     </row>
     <row r="36" spans="1:6" ht="16" customHeight="1">
-      <c r="A36" s="45">
+      <c r="A36" s="36">
         <v>7</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="57"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
     </row>
     <row r="37" spans="1:6" ht="16" customHeight="1">
-      <c r="A37" s="45">
+      <c r="A37" s="36">
         <v>8</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
     </row>
     <row r="38" spans="1:6" ht="16" customHeight="1">
-      <c r="A38" s="45">
+      <c r="A38" s="36">
         <v>9</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="57"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
     </row>
     <row r="39" spans="1:6" ht="16" customHeight="1">
-      <c r="A39" s="44">
+      <c r="A39" s="35">
         <v>10</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42" t="s">
+      <c r="B39" s="32"/>
+      <c r="C39" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
     </row>
     <row r="40" spans="1:6" ht="16" customHeight="1">
-      <c r="A40" s="44">
+      <c r="A40" s="35">
         <v>11</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="42" t="s">
+      <c r="B40" s="32"/>
+      <c r="C40" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="55"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
     </row>
     <row r="41" spans="1:6" ht="16" customHeight="1">
-      <c r="A41" s="45">
+      <c r="A41" s="36">
         <v>12</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="59"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
     </row>
     <row r="42" spans="1:6" ht="16" customHeight="1">
       <c r="A42" s="23"/>
@@ -2465,7 +2619,7 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" ht="29" customHeight="1">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="56" t="s">
         <v>50</v>
       </c>
       <c r="B48" s="27" t="s">
@@ -2479,7 +2633,7 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" ht="29" customHeight="1">
-      <c r="A49" s="39"/>
+      <c r="A49" s="57"/>
       <c r="B49" s="28" t="s">
         <v>53</v>
       </c>
@@ -2491,7 +2645,7 @@
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" ht="29" customHeight="1">
-      <c r="A50" s="40"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="28" t="s">
         <v>55</v>
       </c>
@@ -2503,7 +2657,7 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" ht="16" customHeight="1">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="52" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="28" t="s">
@@ -2517,21 +2671,21 @@
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A52" s="35"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="27" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="59" t="s">
         <v>62</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A53" s="36"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="27" t="s">
         <v>63</v>
       </c>
@@ -2543,7 +2697,7 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A54" s="37"/>
+      <c r="A54" s="55"/>
       <c r="B54" s="27" t="s">
         <v>65</v>
       </c>
@@ -2555,7 +2709,7 @@
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" ht="16" customHeight="1">
-      <c r="A55" s="30"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
       <c r="D55" s="3"/>
@@ -2579,7 +2733,9 @@
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" ht="16" customHeight="1">
-      <c r="A58" s="3"/>
+      <c r="A58" s="62" t="s">
+        <v>71</v>
+      </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2587,25 +2743,31 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="16" customHeight="1">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
+      <c r="A59" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="60" t="s">
+        <v>70</v>
+      </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" ht="16" customHeight="1">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
+      <c r="A60" s="64"/>
+      <c r="B60" s="60" t="s">
+        <v>72</v>
+      </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6" ht="29" customHeight="1">
-      <c r="A61" s="3"/>
-      <c r="B61" s="31" t="s">
-        <v>67</v>
+      <c r="A61" s="65"/>
+      <c r="B61" s="60" t="s">
+        <v>73</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2613,39 +2775,51 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="16" customHeight="1">
-      <c r="A62" s="3"/>
-      <c r="B62" s="25"/>
+      <c r="A62" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="60" t="s">
+        <v>75</v>
+      </c>
       <c r="C62" s="3"/>
       <c r="D62" s="25"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:6" ht="16" customHeight="1">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
+      <c r="A63" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="60" t="s">
+        <v>78</v>
+      </c>
       <c r="C63" s="3"/>
-      <c r="D63" s="32"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="16" customHeight="1">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
+      <c r="A64" s="64"/>
+      <c r="B64" s="60" t="s">
+        <v>79</v>
+      </c>
       <c r="C64" s="3"/>
-      <c r="D64" s="33"/>
+      <c r="D64" s="31"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="16" customHeight="1">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
+      <c r="A65" s="66"/>
+      <c r="B65" s="60" t="s">
+        <v>80</v>
+      </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" ht="16" customHeight="1">
-      <c r="A66" s="3"/>
+      <c r="A66" s="29"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="25"/>
@@ -2685,16 +2859,20 @@
       <c r="F70" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A63:A65"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1"/>
     <hyperlink ref="C52" r:id="rId2"/>
+    <hyperlink ref="D52" r:id="rId3"/>
+    <hyperlink ref="B64" r:id="rId4" display="https://l.facebook.com/l.php?u=http%3A%2F%2Fansm.sante.fr%2FL-ANSM%2FMedicaments-de-therapie-innovante-et-preparations-cellulaires-a-finalite-therapeutique%2FLes-medicaments-de-therapie-innovante-MTI-ATMP%2F(offset)%2F4&amp;h=ATM0adeUTgJ0Wb4W3M5Oc6ztAY6aNjGUAs3eMZpHm5wIAAOqqbtZ1x5glJFQlDZzUI3VkLejmhPI3PRH7AihQe9MNjFvSYCfZNIgl3FfkzwpTIdz1Mk"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>